<commit_message>
test resources updated. all tests passing. data reformatted
</commit_message>
<xml_diff>
--- a/tests/resources/contact_info_master_3_2019.xlsx
+++ b/tests/resources/contact_info_master_3_2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t xml:space="preserve">Re-baseline HMT benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DfT Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDC approval point</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -819,6 +825,16 @@
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
       <c r="D24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="1046585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
started refactor of tests
</commit_message>
<xml_diff>
--- a/tests/resources/contact_info_master_3_2019.xlsx
+++ b/tests/resources/contact_info_master_3_2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t xml:space="preserve">IPDC approval point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMPP - IPA ID Number</t>
   </si>
 </sst>
 </file>
@@ -834,6 +837,11 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="1046585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>